<commit_message>
Finishing all the key features of the website (advanced logic not configured yet)
</commit_message>
<xml_diff>
--- a/backend/downloads/job_responsibilities_template.xlsx
+++ b/backend/downloads/job_responsibilities_template.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -410,16 +410,7 @@
         <v>nama_job</v>
       </c>
       <c r="C1" t="str">
-        <v>job_prefix</v>
-      </c>
-      <c r="D1" t="str">
-        <v>company_code</v>
-      </c>
-      <c r="E1" t="str">
-        <v>band</v>
-      </c>
-      <c r="F1" t="str">
-        <v>flag_mgr</v>
+        <v>deskripsi</v>
       </c>
     </row>
     <row r="2">
@@ -432,19 +423,10 @@
       <c r="C2" t="str">
         <v/>
       </c>
-      <c r="D2" t="str">
-        <v/>
-      </c>
-      <c r="E2" t="str">
-        <v/>
-      </c>
-      <c r="F2" t="str">
-        <v/>
-      </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>